<commit_message>
check op bewerkingen in publicatie vanuit database
</commit_message>
<xml_diff>
--- a/tabellen/concept/5.1/objectentabellen/objecten-concept-5.1-GW.xlsx
+++ b/tabellen/concept/5.1/objectentabellen/objecten-concept-5.1-GW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingcrow-my.sharepoint.com/personal/elisabeth_devries_crow_nl/Documents/Documents/GitHub/NLCS/tabellen/concept/5.1/objectentabellen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{9F36E449-A0ED-4785-AA65-7600C02B25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C07E7047-277A-4263-81B4-E165D7F5D525}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{9F36E449-A0ED-4785-AA65-7600C02B25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4EDB141-414C-49F0-BD90-DE8787A0D4E9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{ADC21C3E-1A3C-46F3-8347-C9E87346AC01}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{ADC21C3E-1A3C-46F3-8347-C9E87346AC01}"/>
   </bookViews>
   <sheets>
     <sheet name="objecten-concept-5.1-GW-algemee" sheetId="1" r:id="rId1"/>
@@ -2595,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48423839-A884-4ED0-A959-D42787D118E6}">
   <dimension ref="A1:BG145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>